<commit_message>
Add correlation between cliff point and emergency date
</commit_message>
<xml_diff>
--- a/data/emergency_date/date_emergency.xlsx
+++ b/data/emergency_date/date_emergency.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Washington</t>
   </si>
@@ -163,6 +163,15 @@
   </si>
   <si>
     <t>missouri</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Difference</t>
   </si>
 </sst>
 </file>
@@ -198,9 +207,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,735 +491,558 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.140625" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B2" s="1">
         <v>43890</v>
       </c>
-      <c r="C1" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D1">
-        <f>B1-C1</f>
+      <c r="C2" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B3" s="1">
         <v>43894</v>
       </c>
-      <c r="C2" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D2">
-        <f t="shared" ref="D2:D48" si="0">B2-C2</f>
+      <c r="C3" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="1">
         <v>43895</v>
       </c>
-      <c r="C3" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D3">
-        <f t="shared" si="0"/>
+      <c r="C4" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>30</v>
-      </c>
-      <c r="B4" s="1">
-        <v>43896</v>
-      </c>
-      <c r="C4" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
       </c>
       <c r="B5" s="1">
         <v>43896</v>
       </c>
-      <c r="C5" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
+      <c r="C5" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1">
+        <v>43896</v>
+      </c>
+      <c r="C6" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="1">
-        <v>43903</v>
-      </c>
-      <c r="C6" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" s="1">
+        <v>43903</v>
+      </c>
+      <c r="C7" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B8" s="1">
         <v>43897</v>
       </c>
-      <c r="C7" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
+      <c r="C8" s="2">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B9" s="1">
         <v>43898</v>
       </c>
-      <c r="C8" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
+      <c r="C9" s="2">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B10" s="1">
         <v>43896</v>
       </c>
-      <c r="C9" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
+      <c r="C10" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B11" s="1">
         <v>43899</v>
       </c>
-      <c r="C10" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
+      <c r="C11" s="2">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B12" s="1">
         <v>43900</v>
       </c>
-      <c r="C11" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
+      <c r="C12" s="2">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>14</v>
-      </c>
-      <c r="B12" s="1">
-        <v>43899</v>
-      </c>
-      <c r="C12" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>36</v>
       </c>
       <c r="B13" s="1">
         <v>43899</v>
       </c>
-      <c r="C13" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
+      <c r="C13" s="2">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="1">
+        <v>43899</v>
+      </c>
+      <c r="C14" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B15" s="1">
         <v>43896</v>
       </c>
-      <c r="C14" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
+      <c r="C15" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B16" s="1">
         <v>43899</v>
       </c>
-      <c r="C15" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
+      <c r="C16" s="2">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>17</v>
-      </c>
-      <c r="B16" s="1">
-        <v>43900</v>
-      </c>
-      <c r="C16" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>40</v>
       </c>
       <c r="B17" s="1">
         <v>43900</v>
       </c>
-      <c r="C17" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
+      <c r="C17" s="2">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="B18" s="1">
         <v>43900</v>
       </c>
-      <c r="C18" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="0"/>
+      <c r="C18" s="2">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B19" s="1">
+        <v>43900</v>
+      </c>
+      <c r="C19" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="1">
         <v>43901</v>
       </c>
-      <c r="C19" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
+      <c r="C20" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B21" s="1">
         <v>43900</v>
       </c>
-      <c r="C20" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="0"/>
+      <c r="C21" s="2">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B22" s="1">
         <v>43901</v>
       </c>
-      <c r="C21" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="0"/>
+      <c r="C22" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>21</v>
-      </c>
-      <c r="B22" s="1">
-        <v>43902</v>
-      </c>
-      <c r="C22" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>37</v>
       </c>
       <c r="B23" s="1">
         <v>43902</v>
       </c>
-      <c r="C23" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="0"/>
+      <c r="C23" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B24" s="1">
         <v>43902</v>
       </c>
-      <c r="C24" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="0"/>
+      <c r="C24" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="B25" s="1">
         <v>43902</v>
       </c>
-      <c r="C25" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="0"/>
+      <c r="C25" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="1">
+        <v>43902</v>
+      </c>
+      <c r="C26" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B27" s="1">
         <v>43901</v>
       </c>
-      <c r="C26" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D26">
-        <f t="shared" si="0"/>
+      <c r="C27" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>23</v>
-      </c>
-      <c r="B27" s="1">
-        <v>43902</v>
-      </c>
-      <c r="C27" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D27">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>16</v>
       </c>
       <c r="B28" s="1">
         <v>43902</v>
       </c>
-      <c r="C28" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D28">
-        <f t="shared" si="0"/>
+      <c r="C28" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="1">
+        <v>43902</v>
+      </c>
+      <c r="C29" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B30" s="1">
         <v>43895</v>
       </c>
-      <c r="C29" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D29">
-        <f t="shared" si="0"/>
+      <c r="C30" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B31" s="1">
         <v>43902</v>
       </c>
-      <c r="C30" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D30">
-        <f t="shared" si="0"/>
+      <c r="C31" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="1">
-        <v>43903</v>
-      </c>
-      <c r="C31" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D31">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="B32" s="1">
+        <v>43903</v>
+      </c>
+      <c r="C32" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="1">
-        <v>43903</v>
-      </c>
-      <c r="C32" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D32">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="B33" s="1">
+        <v>43903</v>
+      </c>
+      <c r="C33" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>45</v>
       </c>
-      <c r="B33" s="1">
-        <v>43903</v>
-      </c>
-      <c r="C33" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D33">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="B34" s="1">
+        <v>43903</v>
+      </c>
+      <c r="C34" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="1">
-        <v>43903</v>
-      </c>
-      <c r="C34" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D34">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="B35" s="1">
+        <v>43903</v>
+      </c>
+      <c r="C35" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>18</v>
       </c>
-      <c r="B35" s="1">
-        <v>43903</v>
-      </c>
-      <c r="C35" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D35">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="B36" s="1">
+        <v>43903</v>
+      </c>
+      <c r="C36" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>47</v>
       </c>
-      <c r="B36" s="1">
-        <v>43903</v>
-      </c>
-      <c r="C36" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D36">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B37" s="1">
+        <v>43903</v>
+      </c>
+      <c r="C37" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>5</v>
       </c>
-      <c r="B37" s="1">
-        <v>43903</v>
-      </c>
-      <c r="C37" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D37">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="B38" s="1">
+        <v>43903</v>
+      </c>
+      <c r="C38" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>32</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B39" s="1">
         <v>43904</v>
       </c>
-      <c r="C38" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D38">
-        <f t="shared" si="0"/>
+      <c r="C39" s="2">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B40" s="1">
         <v>43899</v>
       </c>
-      <c r="C39" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D39">
-        <f t="shared" si="0"/>
+      <c r="C40" s="2">
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>13</v>
-      </c>
-      <c r="B40" s="1">
-        <v>43901</v>
-      </c>
-      <c r="C40" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D40">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>3</v>
       </c>
       <c r="B41" s="1">
         <v>43901</v>
       </c>
-      <c r="C41" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D41">
-        <f t="shared" si="0"/>
+      <c r="C41" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" s="1">
+        <v>43901</v>
+      </c>
+      <c r="C42" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>43</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B43" s="1">
         <v>43904</v>
       </c>
-      <c r="C42" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D42">
-        <f t="shared" si="0"/>
+      <c r="C43" s="2">
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>6</v>
       </c>
-      <c r="B43" s="1">
-        <v>43903</v>
-      </c>
-      <c r="C43" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D43">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="B44" s="1">
+        <v>43903</v>
+      </c>
+      <c r="C44" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>15</v>
       </c>
-      <c r="B44" s="1">
-        <v>43903</v>
-      </c>
-      <c r="C44" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D44">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="B45" s="1">
+        <v>43903</v>
+      </c>
+      <c r="C45" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>25</v>
       </c>
-      <c r="B45" s="1">
-        <v>43903</v>
-      </c>
-      <c r="C45" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D45">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="B46" s="1">
+        <v>43903</v>
+      </c>
+      <c r="C46" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>8</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B47" s="1">
         <v>43905</v>
       </c>
-      <c r="C46" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D46">
-        <f t="shared" si="0"/>
+      <c r="C47" s="2">
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>2</v>
       </c>
-      <c r="B47" s="1">
-        <v>43903</v>
-      </c>
-      <c r="C47" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D47">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="B48" s="1">
+        <v>43903</v>
+      </c>
+      <c r="C48" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>38</v>
       </c>
-      <c r="B48" s="1">
-        <v>43903</v>
-      </c>
-      <c r="C48" s="1">
-        <v>43876</v>
-      </c>
-      <c r="D48">
-        <f t="shared" si="0"/>
+      <c r="B49" s="1">
+        <v>43903</v>
+      </c>
+      <c r="C49" s="2">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>